<commit_message>
DATABASE: fixed wrong quality listed in excel format
</commit_message>
<xml_diff>
--- a/resources/database/data/db_anime - staging data.xlsx
+++ b/resources/database/data/db_anime - staging data.xlsx
@@ -2742,8 +2742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C221" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J244" sqref="J244"/>
+    <sheetView tabSelected="1" topLeftCell="A204" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C218" sqref="C218:C241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13552,7 +13552,7 @@
         <v>0</v>
       </c>
       <c r="C218" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D218" t="s">
         <v>325</v>
@@ -13596,7 +13596,7 @@
         <v>0</v>
       </c>
       <c r="C219" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D219" t="s">
         <v>328</v>
@@ -13641,7 +13641,7 @@
         <v>0</v>
       </c>
       <c r="C220" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D220" t="s">
         <v>353</v>
@@ -13694,7 +13694,7 @@
         <v>0</v>
       </c>
       <c r="C221" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D221" t="s">
         <v>496</v>
@@ -13733,7 +13733,7 @@
         <v>0</v>
       </c>
       <c r="C222" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D222" t="s">
         <v>497</v>
@@ -13777,7 +13777,7 @@
         <v>0</v>
       </c>
       <c r="C223" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D223" t="s">
         <v>498</v>
@@ -13813,7 +13813,7 @@
         <v>0</v>
       </c>
       <c r="C224" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D224" t="s">
         <v>499</v>
@@ -13849,7 +13849,7 @@
         <v>0</v>
       </c>
       <c r="C225" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D225" t="s">
         <v>500</v>
@@ -13885,7 +13885,7 @@
         <v>0</v>
       </c>
       <c r="C226" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D226" t="s">
         <v>369</v>
@@ -13935,7 +13935,7 @@
         <v>0</v>
       </c>
       <c r="C227" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D227" t="s">
         <v>501</v>
@@ -13980,7 +13980,7 @@
         <v>0</v>
       </c>
       <c r="C228" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D228" t="s">
         <v>511</v>
@@ -14025,7 +14025,7 @@
         <v>0</v>
       </c>
       <c r="C229" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D229" t="s">
         <v>503</v>
@@ -14073,7 +14073,7 @@
         <v>0</v>
       </c>
       <c r="C230" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D230" t="s">
         <v>504</v>
@@ -14121,7 +14121,7 @@
         <v>0</v>
       </c>
       <c r="C231" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D231" t="s">
         <v>505</v>
@@ -14169,7 +14169,7 @@
         <v>0</v>
       </c>
       <c r="C232" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D232" t="s">
         <v>380</v>
@@ -14210,7 +14210,7 @@
         <v>0</v>
       </c>
       <c r="C233" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D233" t="s">
         <v>384</v>
@@ -14260,7 +14260,7 @@
         <v>0</v>
       </c>
       <c r="C234" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D234" t="s">
         <v>387</v>
@@ -14308,7 +14308,7 @@
         <v>0</v>
       </c>
       <c r="C235" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D235" t="s">
         <v>390</v>
@@ -14352,7 +14352,7 @@
         <v>0</v>
       </c>
       <c r="C236" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D236" t="s">
         <v>402</v>
@@ -14397,7 +14397,7 @@
         <v>0</v>
       </c>
       <c r="C237" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D237" t="s">
         <v>506</v>
@@ -14442,7 +14442,7 @@
         <v>0</v>
       </c>
       <c r="C238" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D238" t="s">
         <v>421</v>
@@ -14487,7 +14487,7 @@
         <v>0</v>
       </c>
       <c r="C239" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D239" t="s">
         <v>422</v>
@@ -14532,7 +14532,7 @@
         <v>0</v>
       </c>
       <c r="C240" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D240" t="s">
         <v>424</v>
@@ -14577,7 +14577,7 @@
         <v>0</v>
       </c>
       <c r="C241" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D241" t="s">
         <v>507</v>

</xml_diff>